<commit_message>
Commit 6 - Clean code
</commit_message>
<xml_diff>
--- a/Deliverables/Pre-Proposal/project calendar.xlsx
+++ b/Deliverables/Pre-Proposal/project calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renzocastagnino/Documents/Master Data Science/Semester 4/Capstone/Capstone_Project/Deliverables/Pre-Proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F4973D-F752-444E-8439-15E9A482326C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92272654-7799-814B-84AC-0EE515AF751F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21020" xr2:uid="{475C6839-6031-7642-B332-32DFFDC7DEB1}"/>
   </bookViews>
@@ -38,18 +38,12 @@
     <t>Final Proposal Report</t>
   </si>
   <si>
-    <t>Preliminari Presentation</t>
-  </si>
-  <si>
     <t>Mock Presentation</t>
   </si>
   <si>
     <t>Final Project Presentation and Journal Submission</t>
   </si>
   <si>
-    <t>VGG16 Model Implementation</t>
-  </si>
-  <si>
     <t>SHAP Model Implementation</t>
   </si>
   <si>
@@ -72,6 +66,12 @@
   </si>
   <si>
     <t>Tasks</t>
+  </si>
+  <si>
+    <t>Preliminary Presentation</t>
+  </si>
+  <si>
+    <t>VGG16, ResNet , and  Inception Implementation</t>
   </si>
 </sst>
 </file>
@@ -102,18 +102,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -123,18 +117,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,16 +151,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -176,12 +221,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,265 +561,266 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C3C499-3066-7043-9927-F8C94DD361A1}">
   <dimension ref="B4:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="6" width="8.33203125" customWidth="1"/>
+    <col min="4" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="18" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
     <col min="8" max="12" width="9.33203125" customWidth="1"/>
     <col min="13" max="13" width="6.1640625" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" s="7" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6">
+    <row r="4" spans="2:14" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5">
         <v>44095</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>44102</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="9">
         <v>44109</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="15">
         <v>44116</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="13">
         <v>44123</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>44130</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>44137</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>44144</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>44151</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>44158</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>44165</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>44172</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="8" t="s">
-        <v>1</v>
+      <c r="E5" s="10"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="C7" s="7"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="7"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="8"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
-      <c r="C15" s="8"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
-      <c r="C16" s="8"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Commit 8 - model revisioned
</commit_message>
<xml_diff>
--- a/Deliverables/Pre-Proposal/project calendar.xlsx
+++ b/Deliverables/Pre-Proposal/project calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renzocastagnino/Documents/Master Data Science/Semester 4/Capstone/Capstone_Project/Deliverables/Pre-Proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92272654-7799-814B-84AC-0EE515AF751F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234E2532-E0A4-ED49-BEA8-BFFADA2DD9C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21020" xr2:uid="{475C6839-6031-7642-B332-32DFFDC7DEB1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20960" xr2:uid="{475C6839-6031-7642-B332-32DFFDC7DEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -221,30 +221,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +561,7 @@
   <dimension ref="B4:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,7 +569,7 @@
     <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" customWidth="1"/>
     <col min="4" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="13" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
     <col min="8" max="12" width="9.33203125" customWidth="1"/>
     <col min="13" max="13" width="6.1640625" customWidth="1"/>
@@ -587,13 +586,13 @@
       <c r="D4" s="5">
         <v>44102</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>44109</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="11">
         <v>44116</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="10">
         <v>44123</v>
       </c>
       <c r="H4" s="5">
@@ -620,13 +619,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="14" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="1"/>
@@ -634,10 +633,10 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -645,182 +644,182 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="14"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="8"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="16"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="14"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="16"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="16"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="8"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="16"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="14"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="8"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="16"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="8"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="16"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="14"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="8"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="16"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="14"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="3"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="8"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="16"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
-      <c r="C14" s="7"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="14"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="16"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
-      <c r="C15" s="7"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="8"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="16"/>
     </row>
     <row r="16" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
-      <c r="C16" s="7"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="14"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="8"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>